<commit_message>
completed yschool initiation ;DB design modificaions; database name yschool_lite to yschool
</commit_message>
<xml_diff>
--- a/yschool/start_ySchool.xlsx
+++ b/yschool/start_ySchool.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jayrksih\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jayrksih\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -524,6 +524,102 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="AutoShape 4"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -939,7 +1035,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -960,7 +1056,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>43354</v>
+        <v>43355</v>
       </c>
       <c r="B2" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
initial spreadsheet dataloading modifications for grade,division,classroom structure
</commit_message>
<xml_diff>
--- a/yschool/start_ySchool.xlsx
+++ b/yschool/start_ySchool.xlsx
@@ -5,18 +5,21 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\PROJECTS\yschoolnew\yschool\src\main\webapp\spreadsheet-templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\PROJECTS\yschoolnew\yschool\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="6285" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="6285" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="students" sheetId="1" r:id="rId1"/>
-    <sheet name="staffs" sheetId="2" r:id="rId2"/>
-    <sheet name="subjects" sheetId="3" r:id="rId3"/>
-    <sheet name="classes" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet6" sheetId="5" state="hidden" r:id="rId5"/>
+    <sheet name="Grades" sheetId="6" r:id="rId1"/>
+    <sheet name="Divisions" sheetId="7" r:id="rId2"/>
+    <sheet name="Classrooms" sheetId="4" r:id="rId3"/>
+    <sheet name="Subjects" sheetId="3" r:id="rId4"/>
+    <sheet name="Modules" sheetId="8" r:id="rId5"/>
+    <sheet name="Students" sheetId="1" r:id="rId6"/>
+    <sheet name="Staffs" sheetId="2" r:id="rId7"/>
+    <sheet name="Sheet6" sheetId="5" state="hidden" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
@@ -68,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="46">
   <si>
     <t>Addmission No.</t>
   </si>
@@ -109,21 +112,9 @@
     <t>staff No</t>
   </si>
   <si>
-    <t>Subject</t>
-  </si>
-  <si>
-    <t>isoptional</t>
-  </si>
-  <si>
     <t>Grade</t>
   </si>
   <si>
-    <t>Dvision</t>
-  </si>
-  <si>
-    <t>Year</t>
-  </si>
-  <si>
     <t>R.Jaykrish</t>
   </si>
   <si>
@@ -203,6 +194,21 @@
   </si>
   <si>
     <t>Dr Malaka walapola</t>
+  </si>
+  <si>
+    <t>Division</t>
+  </si>
+  <si>
+    <t>Grades</t>
+  </si>
+  <si>
+    <t>Divisions</t>
+  </si>
+  <si>
+    <t>Subject Name</t>
+  </si>
+  <si>
+    <t>isOptional</t>
   </si>
 </sst>
 </file>
@@ -656,6 +662,294 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="AutoShape 4"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="AutoShape 4"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="AutoShape 4"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -921,6 +1215,435 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1024" width="17.28515625"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>7</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Check grade" error="check the grade value you entered." promptTitle="Format" prompt="1 to 13" sqref="A1">
+      <formula1>1</formula1>
+      <formula2>13</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Division" prompt="like a,b,c,d,e..." sqref="B1">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1024" width="17.28515625"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>11</v>
+      </c>
+      <c r="B15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H4"/>
   <sheetViews>
@@ -980,10 +1703,10 @@
         <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="G2">
         <v>10</v>
@@ -997,25 +1720,25 @@
         <v>344234</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="G3">
         <v>10</v>
       </c>
       <c r="H3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -1023,25 +1746,25 @@
         <v>342423</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="G4">
         <v>10</v>
       </c>
       <c r="H4" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1066,7 +1789,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -1095,10 +1818,10 @@
         <v>43354</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1106,10 +1829,10 @@
         <v>12345</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1117,10 +1840,10 @@
         <v>34567</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1129,268 +1852,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1025" width="17.28515625"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>40</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Optional Subject?" error="check the data you entered." promptTitle="Format" prompt="enter 1 if the subject is optional- subject, otherwise leave it blank." sqref="B1">
-      <formula1>0</formula1>
-      <formula2>1</formula2>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C13"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1025" width="17.28515625"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2">
-        <v>2013</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3">
-        <v>2013</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4">
-        <v>2013</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5">
-        <v>2013</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6">
-        <v>2013</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>10</v>
-      </c>
-      <c r="B7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7">
-        <v>2013</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>11</v>
-      </c>
-      <c r="B8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8">
-        <v>2013</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>11</v>
-      </c>
-      <c r="B9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9">
-        <v>2013</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>11</v>
-      </c>
-      <c r="B10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C10">
-        <v>2013</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>11</v>
-      </c>
-      <c r="B11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11">
-        <v>2013</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12">
-        <v>2013</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13">
-        <v>2013</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Check grade" error="check the grade value you entered." promptTitle="Format" prompt="1 to 13" sqref="A1">
-      <formula1>1</formula1>
-      <formula2>13</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Division" prompt="like a,b,c,d,e..." sqref="B1">
-      <formula1>0</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>